<commit_message>
[맘파] ObjectTable Type 수정
</commit_message>
<xml_diff>
--- a/ExcelConverter/ExcelFiles/ObjectTable.xlsx
+++ b/ExcelConverter/ExcelFiles/ObjectTable.xlsx
@@ -8343,8 +8343,8 @@
       <c r="B3" s="11" t="s">
         <v>463</v>
       </c>
-      <c r="C3" s="1">
-        <v>0.0</v>
+      <c r="C3" s="11">
+        <v>2.0</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>464</v>
@@ -8389,8 +8389,8 @@
       <c r="B5" s="11" t="s">
         <v>469</v>
       </c>
-      <c r="C5" s="1">
-        <v>0.0</v>
+      <c r="C5" s="11">
+        <v>2.0</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>470</v>
@@ -8458,8 +8458,8 @@
       <c r="B8" s="11" t="s">
         <v>478</v>
       </c>
-      <c r="C8" s="1">
-        <v>0.0</v>
+      <c r="C8" s="11">
+        <v>2.0</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>479</v>
@@ -8481,8 +8481,8 @@
       <c r="B9" s="11" t="s">
         <v>480</v>
       </c>
-      <c r="C9" s="1">
-        <v>0.0</v>
+      <c r="C9" s="11">
+        <v>2.0</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>481</v>

</xml_diff>

<commit_message>
[맘파]ObjectTable 칼럼 추가, Type 수정
</commit_message>
<xml_diff>
--- a/ExcelConverter/ExcelFiles/ObjectTable.xlsx
+++ b/ExcelConverter/ExcelFiles/ObjectTable.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="501">
   <si>
     <t>테이블 용도: 요리 관련 오브젝트의 데이터를 관리하는 테이블</t>
   </si>
@@ -1410,6 +1410,9 @@
     <t>ToolTimer</t>
   </si>
   <si>
+    <t>OuputFood</t>
+  </si>
+  <si>
     <t>float[]</t>
   </si>
   <si>
@@ -1507,6 +1510,9 @@
   </si>
   <si>
     <t>요리 투입구</t>
+  </si>
+  <si>
+    <t>FoodDeliveryToolObject</t>
   </si>
   <si>
     <t>Table</t>
@@ -8315,6 +8321,9 @@
       <c r="G1" s="11" t="s">
         <v>461</v>
       </c>
+      <c r="H1" s="11" t="s">
+        <v>462</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="11" t="s">
@@ -8333,7 +8342,10 @@
         <v>26</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>462</v>
+        <v>463</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3">
@@ -8341,22 +8353,25 @@
         <v>1001.0</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C3" s="11">
         <v>2.0</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>466</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>464</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>465</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>463</v>
-      </c>
       <c r="G3" s="11" t="s">
-        <v>466</v>
+        <v>467</v>
+      </c>
+      <c r="H3" s="11">
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
@@ -8364,22 +8379,25 @@
         <v>1002.0</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C4" s="11">
         <v>2.0</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>466</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>468</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>465</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>467</v>
       </c>
       <c r="G4" s="11">
         <v>5.0</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
@@ -8387,22 +8405,25 @@
         <v>1003.0</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C5" s="11">
         <v>2.0</v>
       </c>
       <c r="D5" s="11" t="s">
+        <v>471</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>466</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>470</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>465</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>469</v>
-      </c>
       <c r="G5" s="11" t="s">
-        <v>471</v>
+        <v>472</v>
+      </c>
+      <c r="H5" s="11">
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
@@ -8410,22 +8431,25 @@
         <v>1004.0</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C6" s="11">
         <v>4.0</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>475</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>473</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>474</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>472</v>
-      </c>
       <c r="G6" s="11" t="s">
-        <v>475</v>
+        <v>476</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0.0</v>
       </c>
     </row>
     <row r="7">
@@ -8433,22 +8457,25 @@
         <v>1005.0</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C7" s="11">
         <v>4.0</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>475</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>477</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>474</v>
-      </c>
-      <c r="F7" s="11" t="s">
+      <c r="G7" s="11" t="s">
         <v>476</v>
       </c>
-      <c r="G7" s="11" t="s">
-        <v>475</v>
+      <c r="H7" s="11">
+        <v>0.0</v>
       </c>
     </row>
     <row r="8">
@@ -8456,22 +8483,25 @@
         <v>1006.0</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C8" s="11">
         <v>2.0</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>466</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>479</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>465</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>478</v>
-      </c>
       <c r="G8" s="11" t="s">
-        <v>466</v>
+        <v>467</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0.0</v>
       </c>
     </row>
     <row r="9">
@@ -8479,22 +8509,25 @@
         <v>1007.0</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C9" s="11">
         <v>2.0</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>466</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>481</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>465</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>480</v>
-      </c>
       <c r="G9" s="11" t="s">
-        <v>471</v>
+        <v>472</v>
+      </c>
+      <c r="H9" s="11">
+        <v>0.0</v>
       </c>
     </row>
     <row r="10">
@@ -8502,22 +8535,25 @@
         <v>1008.0</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C10" s="11">
         <v>1.0</v>
       </c>
       <c r="D10" s="11" t="s">
+        <v>484</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>485</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>483</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>484</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>482</v>
       </c>
       <c r="G10" s="11">
         <v>0.0</v>
+      </c>
+      <c r="H10" s="11">
+        <v>10.0</v>
       </c>
     </row>
     <row r="11">
@@ -8525,22 +8561,25 @@
         <v>1009.0</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C11" s="11">
         <v>1.0</v>
       </c>
       <c r="D11" s="11" t="s">
+        <v>487</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>485</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>486</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>484</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>485</v>
       </c>
       <c r="G11" s="11">
         <v>0.0</v>
+      </c>
+      <c r="H11" s="11">
+        <v>12.0</v>
       </c>
     </row>
     <row r="12">
@@ -8548,22 +8587,25 @@
         <v>1010.0</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C12" s="11">
         <v>1.0</v>
       </c>
       <c r="D12" s="11" t="s">
+        <v>489</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>485</v>
+      </c>
+      <c r="F12" s="11" t="s">
         <v>488</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>484</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>487</v>
       </c>
       <c r="G12" s="11">
         <v>0.0</v>
+      </c>
+      <c r="H12" s="11">
+        <v>14.0</v>
       </c>
     </row>
     <row r="13">
@@ -8571,22 +8613,25 @@
         <v>1011.0</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C13" s="11">
         <v>1.0</v>
       </c>
       <c r="D13" s="11" t="s">
+        <v>491</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>485</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>490</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>484</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>489</v>
       </c>
       <c r="G13" s="11">
         <v>0.0</v>
+      </c>
+      <c r="H13" s="11">
+        <v>9.0</v>
       </c>
     </row>
     <row r="14">
@@ -8594,22 +8639,25 @@
         <v>1012.0</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C14" s="11">
         <v>1.0</v>
       </c>
       <c r="D14" s="11" t="s">
+        <v>493</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>485</v>
+      </c>
+      <c r="F14" s="11" t="s">
         <v>492</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>484</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>491</v>
       </c>
       <c r="G14" s="11">
         <v>0.0</v>
+      </c>
+      <c r="H14" s="11">
+        <v>16.0</v>
       </c>
     </row>
     <row r="15">
@@ -8617,21 +8665,24 @@
         <v>1013.0</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C15" s="11">
+        <v>5.0</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>495</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>496</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>494</v>
+      </c>
+      <c r="G15" s="11">
         <v>0.0</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>494</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>493</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>493</v>
-      </c>
-      <c r="G15" s="11">
+      <c r="H15" s="11">
         <v>0.0</v>
       </c>
     </row>
@@ -8640,21 +8691,24 @@
         <v>1014.0</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="C16" s="11">
         <v>0.0</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="G16" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="H16" s="11">
         <v>0.0</v>
       </c>
     </row>
@@ -8663,22 +8717,25 @@
         <v>1015.0</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="C17" s="11">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>497</v>
+        <v>485</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="G17" s="11">
         <v>0.0</v>
+      </c>
+      <c r="H17" s="11">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[맘파] ObjectTable ToolObject 에 Animation 추가
</commit_message>
<xml_diff>
--- a/ExcelConverter/ExcelFiles/ObjectTable.xlsx
+++ b/ExcelConverter/ExcelFiles/ObjectTable.xlsx
@@ -13,14 +13,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="rnoxPd2++NEzClqZ25FMLaYYG7qbUnjulSihMUqXyak="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="Vk/GHhmO1Dzl6lOVSxwD66rdkZYk/wxrAzcY+Sgg8/0="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="507">
   <si>
     <t>테이블 용도: 요리 관련 오브젝트의 데이터를 관리하는 테이블</t>
   </si>
@@ -1416,6 +1416,9 @@
     <t>ToolTimer</t>
   </si>
   <si>
+    <t>Animation</t>
+  </si>
+  <si>
     <t>OutputFood</t>
   </si>
   <si>
@@ -1434,10 +1437,16 @@
     <t>9,18</t>
   </si>
   <si>
+    <t>Hold</t>
+  </si>
+  <si>
     <t>Board</t>
   </si>
   <si>
     <t>도마</t>
+  </si>
+  <si>
+    <t>Chop</t>
   </si>
   <si>
     <t>Mixer</t>
@@ -8349,6 +8358,9 @@
       <c r="H1" s="10" t="s">
         <v>464</v>
       </c>
+      <c r="I1" s="10" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="10" t="s">
@@ -8367,9 +8379,12 @@
         <v>28</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="H2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>27</v>
       </c>
     </row>
@@ -8378,24 +8393,27 @@
         <v>1001.0</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C3" s="10">
         <v>2.0</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>469</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>467</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>468</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>466</v>
-      </c>
       <c r="G3" s="10" t="s">
-        <v>469</v>
-      </c>
-      <c r="H3" s="10">
+        <v>470</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="I3" s="10">
         <v>0.0</v>
       </c>
     </row>
@@ -8404,24 +8422,27 @@
         <v>1002.0</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="C4" s="10">
         <v>2.0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="G4" s="10">
         <v>5.0</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="I4" s="10">
         <v>0.0</v>
       </c>
     </row>
@@ -8430,24 +8451,27 @@
         <v>1003.0</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="C5" s="10">
         <v>2.0</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="H5" s="10">
+        <v>477</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="I5" s="10">
         <v>0.0</v>
       </c>
     </row>
@@ -8456,24 +8480,27 @@
         <v>1004.0</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="C6" s="10">
         <v>4.0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>478</v>
-      </c>
-      <c r="H6" s="10">
+        <v>481</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="I6" s="10">
         <v>0.0</v>
       </c>
     </row>
@@ -8482,24 +8509,27 @@
         <v>1005.0</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="C7" s="10">
         <v>4.0</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>480</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>477</v>
-      </c>
       <c r="F7" s="10" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>478</v>
-      </c>
-      <c r="H7" s="10">
+        <v>481</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="I7" s="10">
         <v>0.0</v>
       </c>
     </row>
@@ -8508,24 +8538,27 @@
         <v>1006.0</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="C8" s="10">
         <v>2.0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>469</v>
-      </c>
-      <c r="H8" s="10">
+        <v>470</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="I8" s="10">
         <v>0.0</v>
       </c>
     </row>
@@ -8534,24 +8567,27 @@
         <v>1007.0</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="C9" s="10">
         <v>2.0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="H9" s="10">
+        <v>477</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="I9" s="10">
         <v>0.0</v>
       </c>
     </row>
@@ -8560,24 +8596,27 @@
         <v>1008.0</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="C10" s="10">
         <v>1.0</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="G10" s="10">
         <v>0.0</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="I10" s="10">
         <v>10.0</v>
       </c>
     </row>
@@ -8586,24 +8625,27 @@
         <v>1009.0</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="C11" s="10">
         <v>1.0</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="G11" s="10">
         <v>0.0</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="I11" s="10">
         <v>12.0</v>
       </c>
     </row>
@@ -8612,24 +8654,27 @@
         <v>1010.0</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="C12" s="10">
         <v>1.0</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="G12" s="10">
         <v>0.0</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="I12" s="10">
         <v>14.0</v>
       </c>
     </row>
@@ -8638,24 +8683,27 @@
         <v>1011.0</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="C13" s="10">
         <v>1.0</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="G13" s="10">
         <v>0.0</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="I13" s="10">
         <v>9.0</v>
       </c>
     </row>
@@ -8664,24 +8712,27 @@
         <v>1012.0</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="C14" s="10">
         <v>1.0</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="G14" s="10">
         <v>0.0</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="I14" s="10">
         <v>16.0</v>
       </c>
     </row>
@@ -8690,24 +8741,27 @@
         <v>1013.0</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="C15" s="10">
         <v>5.0</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="G15" s="10">
         <v>0.0</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="I15" s="10">
         <v>0.0</v>
       </c>
     </row>
@@ -8716,24 +8770,27 @@
         <v>1014.0</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="C16" s="10">
         <v>3.0</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="G16" s="10">
         <v>0.0</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="I16" s="10">
         <v>0.0</v>
       </c>
     </row>
@@ -8742,24 +8799,27 @@
         <v>1015.0</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="C17" s="10">
         <v>1.0</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="G17" s="10">
         <v>0.0</v>
       </c>
-      <c r="H17" s="10">
+      <c r="H17" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="I17" s="10">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>